<commit_message>
DESCW-1256 build template & menuselector option
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_31_rpt_PA_ProjectswithContracts.xlsx
+++ b/backend/reports/xlsx/Tab_31_rpt_PA_ProjectswithContracts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF112A5-F0EC-304E-8B7F-C7658D65EB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF838B31-830B-4448-A3D2-AC4010D9F71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,16 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>{#r=d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>{#date=d.date}</t>
   </si>
@@ -96,6 +87,96 @@
   <si>
     <t>Contract 
 Version</t>
+  </si>
+  <si>
+    <t>{$r.project_name}</t>
+  </si>
+  <si>
+    <t>{#r=d.repotsByProjectWithTotals[i]}</t>
+  </si>
+  <si>
+    <t>{#r1=d.repotsByProjectWithTotals[i+1]}</t>
+  </si>
+  <si>
+    <t>{#p=d.repotsByProjectWithTotals[i].projects[i]}</t>
+  </si>
+  <si>
+    <t>{#gt=d.grandTotals[0]}</t>
+  </si>
+  <si>
+    <t>{#p1=d.repotsByProjectWithTotals[i].projects[i+1]}</t>
+  </si>
+  <si>
+    <t>{$p.project_number}</t>
+  </si>
+  <si>
+    <t>{$p.project_name}</t>
+  </si>
+  <si>
+    <t>{$p.total_project_budget}</t>
+  </si>
+  <si>
+    <t>{$p.fiscal_year}</t>
+  </si>
+  <si>
+    <t>{$p.contract_number}</t>
+  </si>
+  <si>
+    <t>{$p.co_version}</t>
+  </si>
+  <si>
+    <t>{$p.supplier_subcontractor}</t>
+  </si>
+  <si>
+    <t>{$p.end_date}</t>
+  </si>
+  <si>
+    <t>{$p.total_contract_amount}</t>
+  </si>
+  <si>
+    <t>{$p.invoiced_to_date}</t>
+  </si>
+  <si>
+    <t>{$p.balance_remaining}</t>
+  </si>
+  <si>
+    <t>{$p.descoped}</t>
+  </si>
+  <si>
+    <t>{$p1.project_number}</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>{$p.subtotal_invoiced_to_date}</t>
+  </si>
+  <si>
+    <t>{$p.subtotal_balance_remaining}</t>
+  </si>
+  <si>
+    <t>{$p.subtotal_descoped}</t>
+  </si>
+  <si>
+    <t>{$r1.project_name}</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>{$gt.total_contract_amount}</t>
+  </si>
+  <si>
+    <t>{$p.subtotal_contract_amount}</t>
+  </si>
+  <si>
+    <t>{$gt.invoiced_to_date}</t>
+  </si>
+  <si>
+    <t>{$gt.balance_remaining}</t>
+  </si>
+  <si>
+    <t>{$gt.descoped}</t>
   </si>
 </sst>
 </file>
@@ -105,7 +186,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,8 +222,26 @@
       <color theme="1"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8.5"/>
+      <name val="BCSans-Regular"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,28 +260,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -233,55 +323,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -292,6 +435,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF2F2F2"/>
       <color rgb="FF003365"/>
       <color rgb="FFC5DAF1"/>
     </mruColors>
@@ -318,7 +462,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
+      <xdr:colOff>1137948</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>680356</xdr:rowOff>
     </xdr:to>
@@ -662,147 +806,304 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="161" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="17" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1">
+      <c r="A2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="14"/>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="32">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="33" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="F3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="H3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="I3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="K3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="14"/>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="21">
+      <c r="A12" s="3"/>
+      <c r="B12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="1:12" ht="21">
+      <c r="A13" s="3"/>
+      <c r="B13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="4" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="1:12" ht="21">
+      <c r="A14" s="3"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:12" ht="21">
+      <c r="A15" s="3"/>
+      <c r="B15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+    </row>
+    <row r="16" spans="1:12" ht="21">
+      <c r="A16" s="3"/>
+      <c r="B16" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="1:5" ht="21">
+      <c r="A17" s="3"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="1:5" ht="21">
+      <c r="A18" s="3"/>
+      <c r="B18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="1:5" ht="21">
+      <c r="A19" s="3"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="1:5" ht="21">
+      <c r="A20" s="3"/>
+      <c r="B20" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="1:5" ht="21">
+      <c r="A21" s="3"/>
+      <c r="B21" s="16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
+    <mergeCell ref="A7:L7"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
descw-1256 model returns report JSON with totals
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_31_rpt_PA_ProjectswithContracts.xlsx
+++ b/backend/reports/xlsx/Tab_31_rpt_PA_ProjectswithContracts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF838B31-830B-4448-A3D2-AC4010D9F71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D354F9-CE8C-D04F-8F13-C1CC6F4D4C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-10920" yWindow="-19220" windowWidth="21600" windowHeight="19880" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
+    <t>{#r=d.report[i]}</t>
+  </si>
+  <si>
+    <t>{#r1=d.report[i+1]}</t>
+  </si>
+  <si>
     <t>{#date=d.date}</t>
   </si>
   <si>
@@ -92,19 +98,7 @@
     <t>{$r.project_name}</t>
   </si>
   <si>
-    <t>{#r=d.repotsByProjectWithTotals[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.repotsByProjectWithTotals[i+1]}</t>
-  </si>
-  <si>
-    <t>{#p=d.repotsByProjectWithTotals[i].projects[i]}</t>
-  </si>
-  <si>
-    <t>{#gt=d.grandTotals[0]}</t>
-  </si>
-  <si>
-    <t>{#p1=d.repotsByProjectWithTotals[i].projects[i+1]}</t>
+    <t>{#p=d.report[i].projects[i]}</t>
   </si>
   <si>
     <t>{$p.project_number}</t>
@@ -177,6 +171,12 @@
   </si>
   <si>
     <t>{$gt.descoped}</t>
+  </si>
+  <si>
+    <t>{#p1=d.report[i].projects[i+1]}</t>
+  </si>
+  <si>
+    <t>{#gt=d.totals[0]}</t>
   </si>
 </sst>
 </file>
@@ -808,8 +808,8 @@
   </sheetPr>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="161" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -830,7 +830,7 @@
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -844,7 +844,7 @@
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -860,83 +860,83 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="32">
       <c r="A3" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
       <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="I4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="J4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="L4" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
       <c r="A5" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -959,24 +959,24 @@
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="15" t="s">
+      <c r="L6" s="15" t="s">
         <v>35</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
       <c r="A7" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -999,25 +999,25 @@
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="K8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="21">
       <c r="A12" s="3"/>
       <c r="B12" s="16" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -1026,7 +1026,7 @@
     <row r="13" spans="1:12" ht="21">
       <c r="A13" s="3"/>
       <c r="B13" s="16" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -1051,7 +1051,7 @@
     <row r="16" spans="1:12" ht="21">
       <c r="A16" s="3"/>
       <c r="B16" s="16" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -1067,7 +1067,7 @@
     <row r="18" spans="1:5" ht="21">
       <c r="A18" s="3"/>
       <c r="B18" s="16" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -1083,7 +1083,7 @@
     <row r="20" spans="1:5" ht="21">
       <c r="A20" s="3"/>
       <c r="B20" s="16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -1092,7 +1092,7 @@
     <row r="21" spans="1:5" ht="21">
       <c r="A21" s="3"/>
       <c r="B21" s="16" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>

</xml_diff>

<commit_message>
descw-1256 gets all data populating the template
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_31_rpt_PA_ProjectswithContracts.xlsx
+++ b/backend/reports/xlsx/Tab_31_rpt_PA_ProjectswithContracts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D354F9-CE8C-D04F-8F13-C1CC6F4D4C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F1A1FA-ABB4-414E-B31F-C709CD5BE5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10920" yWindow="-19220" windowWidth="21600" windowHeight="19880" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>{#r=d.report[i]}</t>
   </si>
@@ -113,9 +113,6 @@
     <t>{$p.fiscal_year}</t>
   </si>
   <si>
-    <t>{$p.contract_number}</t>
-  </si>
-  <si>
     <t>{$p.co_version}</t>
   </si>
   <si>
@@ -137,33 +134,15 @@
     <t>{$p.descoped}</t>
   </si>
   <si>
-    <t>{$p1.project_number}</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>{$p.subtotal_invoiced_to_date}</t>
-  </si>
-  <si>
-    <t>{$p.subtotal_balance_remaining}</t>
-  </si>
-  <si>
-    <t>{$p.subtotal_descoped}</t>
-  </si>
-  <si>
-    <t>{$r1.project_name}</t>
-  </si>
-  <si>
     <t>Grand Total</t>
   </si>
   <si>
     <t>{$gt.total_contract_amount}</t>
   </si>
   <si>
-    <t>{$p.subtotal_contract_amount}</t>
-  </si>
-  <si>
     <t>{$gt.invoiced_to_date}</t>
   </si>
   <si>
@@ -176,7 +155,31 @@
     <t>{#p1=d.report[i].projects[i+1]}</t>
   </si>
   <si>
-    <t>{#gt=d.totals[0]}</t>
+    <t>{$p.co_number}</t>
+  </si>
+  <si>
+    <t>{#s=d.report[i].subtotals}</t>
+  </si>
+  <si>
+    <t>{$s.subtotal_total_contract_amount}</t>
+  </si>
+  <si>
+    <t>{$s.subtotal_invoiced_to_date}</t>
+  </si>
+  <si>
+    <t>{$s.subtotal_balance_remaining}</t>
+  </si>
+  <si>
+    <t>{$s.subtotal_descoped}</t>
+  </si>
+  <si>
+    <t>{$r1}</t>
+  </si>
+  <si>
+    <t>{$p1}</t>
+  </si>
+  <si>
+    <t>{#gt=d.totals}</t>
   </si>
 </sst>
 </file>
@@ -186,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,23 +211,12 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
       <sz val="8"/>
-      <color theme="1"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="BCSans-Regular"/>
     </font>
@@ -238,6 +230,11 @@
     <font>
       <b/>
       <sz val="8.5"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="BCSans-Regular"/>
     </font>
   </fonts>
@@ -366,7 +363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -382,13 +379,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -403,28 +400,28 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -806,10 +803,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -820,10 +817,10 @@
     <col min="4" max="6" width="15.83203125" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" customWidth="1"/>
+    <col min="11" max="11" width="25.83203125" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
@@ -910,33 +907,33 @@
         <v>22</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="L4" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -951,156 +948,171 @@
       <c r="L5" s="15"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" ht="19">
+      <c r="A7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="15" t="s">
+      <c r="J8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L8" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A7" s="12" t="s">
+    <row r="9" spans="1:12" ht="19">
+      <c r="A9" s="3"/>
+      <c r="B9" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="1:12" ht="19">
+      <c r="A10" s="3"/>
+      <c r="B10" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:12" ht="19">
+      <c r="A11" s="3"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:12" ht="19">
+      <c r="A12" s="3"/>
+      <c r="B12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:12" ht="19">
+      <c r="A13" s="3"/>
+      <c r="B13" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="14"/>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:12" ht="19">
+      <c r="A14" s="3"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:12" ht="19">
+      <c r="A15" s="3"/>
+      <c r="B15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="21">
-      <c r="A12" s="3"/>
-      <c r="B12" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="1:12" ht="21">
-      <c r="A13" s="3"/>
-      <c r="B13" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="1:12" ht="21">
-      <c r="A14" s="3"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:12" ht="21">
-      <c r="A15" s="3"/>
-      <c r="B15" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16" spans="1:12" ht="21">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:12" ht="19">
       <c r="A16" s="3"/>
-      <c r="B16" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="1:5" ht="21">
+      <c r="B16" s="20"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" ht="19">
       <c r="A17" s="3"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="1:5" ht="21">
+      <c r="B17" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" ht="19">
       <c r="A18" s="3"/>
-      <c r="B18" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="1:5" ht="21">
+      <c r="B18" s="20"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+    </row>
+    <row r="19" spans="1:5" ht="19">
       <c r="A19" s="3"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="1:5" ht="21">
+      <c r="B19" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" ht="19">
       <c r="A20" s="3"/>
-      <c r="B20" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-    </row>
-    <row r="21" spans="1:5" ht="21">
-      <c r="A21" s="3"/>
-      <c r="B21" s="16" t="s">
+      <c r="B20" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A7:L7"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="A2:L2"/>

</xml_diff>

<commit_message>
descw-1279 adds utility for adding report subtotals
* cosmetic fixes to tab 31 template
* extract subtotal utility from Class definition on tab31 model
* refactor subtotal utility for concision
* remove unneded function from utilities
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_31_rpt_PA_ProjectswithContracts.xlsx
+++ b/backend/reports/xlsx/Tab_31_rpt_PA_ProjectswithContracts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145A5EC3-2507-D24D-813B-43BDA80CE43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38ED9FA-4D55-3B4E-8CE0-D91F751025DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -403,8 +403,8 @@
     <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -421,10 +421,7 @@
     <xf numFmtId="4" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -808,8 +805,8 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:L8"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -951,26 +948,26 @@
       <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
       <c r="H6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="L6" s="17" t="s">
         <v>42</v>
       </c>
     </row>
@@ -985,10 +982,10 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
       <c r="A8" s="12"/>
@@ -998,19 +995,19 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="L8" s="17" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1121,7 +1118,7 @@
     <mergeCell ref="A2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="5" scale="55" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddFooter>&amp;LTab_43_rpt_PF_RecoveryForecast
 &amp;C&amp;P of &amp;N&amp;R{$date}</oddFooter>

</xml_diff>